<commit_message>
Don't remember!! Been here after a long time!-_-
</commit_message>
<xml_diff>
--- a/dwdm_1/Comparision.xlsx
+++ b/dwdm_1/Comparision.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t xml:space="preserve">Accuracy</t>
   </si>
@@ -41,6 +41,15 @@
   </si>
   <si>
     <t xml:space="preserve">Median</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decision Tree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70-30-split</t>
   </si>
 </sst>
 </file>
@@ -55,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -136,15 +146,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="310" zoomScaleNormal="310" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="12.780612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -154,6 +164,18 @@
       <c r="C1" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
@@ -165,6 +187,18 @@
       <c r="C2" s="0" t="n">
         <v>0.849</v>
       </c>
+      <c r="D2" s="0" t="n">
+        <v>82.6</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>0.832</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>89.13</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>0.889</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
@@ -176,6 +210,18 @@
       <c r="C3" s="0" t="n">
         <v>0.819</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>69.56</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>0.72</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>80.43</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>0.808</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
@@ -187,6 +233,18 @@
       <c r="C4" s="0" t="n">
         <v>0.865</v>
       </c>
+      <c r="D4" s="0" t="n">
+        <v>82.6</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.789</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>84.78</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>0.844</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
@@ -198,6 +256,18 @@
       <c r="C5" s="0" t="n">
         <v>0.857</v>
       </c>
+      <c r="D5" s="0" t="n">
+        <v>78.26</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.772</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>84.78</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.836</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
@@ -208,6 +278,34 @@
       </c>
       <c r="C6" s="0" t="n">
         <v>0.887</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>80.43</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>0.717</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>82.6</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>0.826</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>